<commit_message>
hcr sequence input enabled
</commit_message>
<xml_diff>
--- a/HCR3_probe_design_files/probes.xlsx
+++ b/HCR3_probe_design_files/probes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,25 +466,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>vip</t>
+          <t>tfrc</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NM_001260752.1</t>
+          <t>NM_011638.4</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>AgCTCAgTCCATCCTCgTtaGGCCTTATTTCTGGTGTCCA</t>
+          <t>AgCTCAgTCCATCCTCgTtaTGATCTGGCTTGATCCATCA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>GTCAGAAGCACAAGGAGCTGatAAATCCTCATCAATCATC</t>
+          <t>CCAAACAAGTTAGAGAATGCatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>
@@ -494,25 +494,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>vip</t>
+          <t>tfrc</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NM_001260752.1</t>
+          <t>NM_011638.4</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>AgCTCAgTCCATCCTCgTtaGTGAGAACAGCACACTGAGA</t>
+          <t>AgCTCAgTCCATCCTCgTtaTGCCGAGCAAGGCTAAACCG</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>AAGAGGCCATGCCGACGTCTatAAATCCTCATCAATCATC</t>
+          <t>GACTGTTATCTCCATCTACTatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>
@@ -522,25 +522,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>vip</t>
+          <t>tfrc</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NM_001260752.1</t>
+          <t>NM_011638.4</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>409</v>
+        <v>283</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>AgCTCAgTCCATCCTCgTtaACTCCATCAGCATGCCTGGC</t>
+          <t>AgCTCAgTCCATCCTCgTtaTTTCTTCTTCATCTGCAGCC</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>TACTGAAGTCACTGGTGAAAatAAATCCTCATCAATCATC</t>
+          <t>CTTCATGTTATTGTCGGCATatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>
@@ -550,25 +550,697 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>vip</t>
+          <t>tfrc</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NM_001260752.1</t>
+          <t>NM_011638.4</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>509</v>
+        <v>339</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>AgCTCAgTCCATCCTCgTtaGTCTTCTGAGATGTTGCTGC</t>
+          <t>AgCTCAgTCCATCCTCgTtaTCTTCCATTAAACCTCTTGG</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>TGACGTTTGACTGGCACAGGatAAATCCTCATCAATCATC</t>
+          <t>GCAATAGCTGCAAAGCAGAGatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>402</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaCAGGTAGCCACTCATGAATC</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>TCTACACGCTTACAATAGCCatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>448</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaCCAGTTTCACACACTCCTCT</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>GTCTGTCTCCTCCGTTTCAGatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>494</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaTCCTCTGTTTCCATGGTTTC</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>AGCGAGATGATGTAGGAACAatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>552</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaCTTCTCTGACAACAGTGTTT</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>GCAAACTCTATGGAGTTCAAatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>598</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaTCTGGCTCAGCTGCTTGATG</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>CTCACGAGGAGTGTATGTATatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>697</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaGCCAGACTTTGCTGAATTTA</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>CTTCACATAGTGTTCATCTCatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>764</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaTGCACTATGGTCACCATGTT</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>GGTCTAAGTTACCATTTGACatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>821</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaTTACTGAATGCCACATAACC</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>TACCAGAAACTTCTGTAGGTatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1035</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaAAGGTCTGCCTCAACAACGG</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>TGAGCATGTCCAAAGAGTGCatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1081</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaGTGTGTATGGATCACCAGTT</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ATTGAAAGAAGGAAAGCCAGatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1132</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaCTGATGACTGAGATGGCGGA</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>CACAGGTATATTAGGCAACCatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1212</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaAGGACAGCTTCCTTCCATTT</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>GAATCTATGTTCCATCTAGCatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1348</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaCTGGTTCCTCATAACCTTTA</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>TCCTACTACAACATAACGGTatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1416</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaCACACTGGACTTCGCCGCAA</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>TTCAACAGAAGACCTGTTCCatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1506</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaGGCAAAGATTATACTTCTGC</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>AAGTCGCCTGCAGTCCAGCTatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1557</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaCTCCAACCACTCAGTGGCAC</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>TGCAAAGATGAAAGGTATCCatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1629</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaACTAGTACCAAGGACAACTT</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>CTGGCAGAAACTTTGAAGTTatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1761</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaGGAAAGTTTCTCAACTTTGC</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>GGATATGCAGCATTGTCAAAatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1852</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaCCAAATAAGGATAGTCTGCA</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>ATAGGTATCCAATCTAGTGCatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1898</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaTGAGGAACTTTCTGAGTCAA</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>TACGAACCATTTGGTTGAGCatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2078</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaAGCCACTGTAGACTTAGACC</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>AGTCTCCACGAGCGGAATACatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2215</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaGCGACAGGAAGTGATACTCC</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>CTCTCTTGGAGATACATAGGatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2279</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaAGAGTGTGAGAGCCAGAGCC</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>AGTTCTCCACTAAAGCTGAGatAAATCCTCATCAATCATC</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>tfrc</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>NM_011638.4</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>2360</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>AgCTCAgTCCATCCTCgTtaGCCAACTGGTTTCTGAAGAG</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>GAATAGTCCAAGTAGCCAGGatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
generating probes against sequence updates
</commit_message>
<xml_diff>
--- a/HCR3_probe_design_files/probes.xlsx
+++ b/HCR3_probe_design_files/probes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,25 +466,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>vegfa</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NM_001317043.1</t>
-        </is>
-      </c>
+          <t>egfp</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>1046</v>
+        <v>51</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CACTTCATATCACTCACTtaGGTACAGCAGTAAAGCCAGG</t>
+          <t>AgCTCAgTCCATCCTCgTtaTTTACGTCGCCGTCCAGCTC</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>GGACCACTTGGCATGGTGGAatCCCAATCTCTATCTACCC</t>
+          <t>ACACGCTGAACTTGTGGCCGatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>
@@ -494,25 +490,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>vegfa</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>NM_001317043.1</t>
-        </is>
-      </c>
+          <t>egfp</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>1123</v>
+        <v>226</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CACTTCATATCACTCACTtaCATGAACTTCACCACTTCAT</t>
+          <t>AgCTCAgTCCATCCTCgTtaGTGCTGCTTCATGTGGTCGG</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>TAGCTGCGCTGGTAGACGTCatCCCAATCTCTATCTACCC</t>
+          <t>ATGGCGGACTTGAAGAAGTCatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>
@@ -522,25 +514,21 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>vegfa</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>NM_001317043.1</t>
-        </is>
-      </c>
+          <t>egfp</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>1187</v>
+        <v>276</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CACTTCATATCACTCACTtaGGTACTCCTGGAAGATGTCC</t>
+          <t>AgCTCAgTCCATCCTCgTtaATGGTGCGCTCCTGGACGTA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>GATATACTCTATCTCATCGGatCCCAATCTCTATCTACCC</t>
+          <t>TGCCGTCGTCCTTGAAGAAGatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>
@@ -550,25 +538,21 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>vegfa</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>NM_001317043.1</t>
-        </is>
-      </c>
+          <t>egfp</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1298</v>
+        <v>361</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CACTTCATATCACTCACTtaTGACGTTGCTCTCCGACGTG</t>
+          <t>AgCTCAgTCCATCCTCgTtaCTTCAGCTCGATGCGGTTCA</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>GATCCGCATGATCTGCATAGatCCCAATCTCTATCTACCC</t>
+          <t>TCCTCCTTGAAGTCGATGCCatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>
@@ -578,25 +562,21 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>vegfa</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NM_001317043.1</t>
-        </is>
-      </c>
+          <t>egfp</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>1344</v>
+        <v>415</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CACTTCATATCACTCACTtaCCTATGTGCTGGCTTTGGTG</t>
+          <t>AgCTCAgTCCATCCTCgTtaGTTGTACTCCAGCTTGTGCC</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>GCTGCAGGAAGCTCATCTCTatCCCAATCTCTATCTACCC</t>
+          <t>TAGACGTTGTGGCTGTTGTAatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>
@@ -606,25 +586,21 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>vegfa</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NM_001317043.1</t>
-        </is>
-      </c>
+          <t>egfp</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>1430</v>
+        <v>461</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CACTTCATATCACTCACTtaAACAAGGCTCACAGTGATTT</t>
+          <t>AgCTCAgTCCATCCTCgTtaCGTTCTTCTGCTTGTCGGCC</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CAAATGCTTTCTCCGCTCTGatCCCAATCTCTATCTACCC</t>
+          <t>CTTGAAGTTCACCTTGATGCatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>
@@ -634,53 +610,21 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>vegfa</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NM_001317043.1</t>
-        </is>
-      </c>
+          <t>egfp</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>1488</v>
+        <v>634</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CACTTCATATCACTCACTtaTTGCAGGAACATTTACACGT</t>
+          <t>AgCTCAgTCCATCCTCgTtaGTGATCGCGCTTCTCGTTGG</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>TGCAACGCGAGTCTGTGTTTatCCCAATCTCTATCTACCC</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>vegfa</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>NM_001317043.1</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>1534</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>CACTTCATATCACTCACTtaTTCGTTTAACTCAAGCTGCC</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>TTGTCACATCTGCAAGTACGatCCCAATCTCTATCTACCC</t>
+          <t>ACGAACTCCAGCAGGACCATatAAATCCTCATCAATCATC</t>
         </is>
       </c>
     </row>

</xml_diff>